<commit_message>
add Student,Discipline - controller and jsp
</commit_message>
<xml_diff>
--- a/doc/действияъ.xlsx
+++ b/doc/действияъ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>№</t>
   </si>
@@ -149,13 +149,43 @@
   </si>
   <si>
     <t>Весь список</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>removeGroup</t>
+  </si>
+  <si>
+    <t>UpdateTerm</t>
+  </si>
+  <si>
+    <t>UpdateGroup</t>
+  </si>
+  <si>
+    <t>UpdateStudentProgress</t>
+  </si>
+  <si>
+    <t>Student Curriculum</t>
+  </si>
+  <si>
+    <t>addCurriculum</t>
+  </si>
+  <si>
+    <t>removeCurriculum</t>
+  </si>
+  <si>
+    <t>findByTerm</t>
+  </si>
+  <si>
+    <t>UpdateCurriculum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +230,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -227,11 +264,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,15 +284,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -564,7 +602,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="6" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -588,7 +626,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="6" tint="-0.249977111117893"/>
+        <color theme="5" tint="0.39997558519241921"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -716,8 +754,8 @@
     <tableColumn id="1" name="№" dataDxfId="16"/>
     <tableColumn id="2" name="Описание" dataDxfId="15"/>
     <tableColumn id="3" name="Сервис" dataDxfId="14"/>
-    <tableColumn id="5" name="Имя метода" dataDxfId="12"/>
-    <tableColumn id="4" name="действие" dataDxfId="13"/>
+    <tableColumn id="5" name="Имя метода" dataDxfId="13"/>
+    <tableColumn id="4" name="действие" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -776,8 +814,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Таблица689" displayName="Таблица689" ref="I22:K25" totalsRowShown="0">
-  <autoFilter ref="I22:K25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Таблица689" displayName="Таблица689" ref="I22:K27" totalsRowShown="0">
+  <autoFilter ref="I22:K27"/>
   <tableColumns count="3">
     <tableColumn id="1" name="№"/>
     <tableColumn id="2" name="Имя метода"/>
@@ -788,8 +826,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Таблица68910" displayName="Таблица68910" ref="I29:K32" totalsRowShown="0">
-  <autoFilter ref="I29:K32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Таблица68910" displayName="Таблица68910" ref="I30:K36" totalsRowShown="0">
+  <autoFilter ref="I30:K36"/>
   <tableColumns count="3">
     <tableColumn id="1" name="№"/>
     <tableColumn id="2" name="Имя метода"/>
@@ -800,8 +838,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Таблица6891011" displayName="Таблица6891011" ref="I35:K37" totalsRowShown="0">
-  <autoFilter ref="I35:K37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Таблица6891011" displayName="Таблица6891011" ref="I48:K53" totalsRowShown="0">
+  <autoFilter ref="I48:K53"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="№"/>
+    <tableColumn id="2" name="Имя метода"/>
+    <tableColumn id="3" name="Описание"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица689103" displayName="Таблица689103" ref="I39:K44" totalsRowShown="0">
+  <autoFilter ref="I39:K44"/>
   <tableColumns count="3">
     <tableColumn id="1" name="№"/>
     <tableColumn id="2" name="Имя метода"/>
@@ -1098,18 +1148,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:K37"/>
+  <dimension ref="B5:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
@@ -1117,16 +1167,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="I6" t="s">
         <v>0</v>
       </c>
@@ -1138,19 +1188,19 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I7">
@@ -1164,19 +1214,19 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I8">
@@ -1190,19 +1240,19 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I9">
@@ -1216,19 +1266,19 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I10">
@@ -1242,19 +1292,19 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="8"/>
       <c r="I11">
         <v>5</v>
       </c>
@@ -1266,29 +1316,29 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="I13" s="1" t="s">
+      <c r="C13" s="10"/>
+      <c r="I13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I14" t="s">
@@ -1302,19 +1352,19 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I15">
@@ -1339,10 +1389,10 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="10"/>
       <c r="I17">
         <v>3</v>
       </c>
@@ -1354,19 +1404,19 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I18">
@@ -1380,19 +1430,19 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I19">
@@ -1406,10 +1456,10 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
@@ -1455,109 +1505,225 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I28" s="1" t="s">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I29" t="s">
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J30" t="s">
         <v>17</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K30" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I34">
         <v>3</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J34" t="s">
         <v>23</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J34" s="1"/>
-    </row>
     <row r="35" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I35" t="s">
-        <v>0</v>
+      <c r="I35">
+        <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" t="s">
         <v>1</v>
       </c>
-      <c r="J36" t="s">
+    </row>
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I47" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
         <v>41</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I37">
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I50">
         <v>2</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J50" t="s">
         <v>42</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K50" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I51" s="11">
+        <v>3</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I52" s="11">
+        <v>4</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="11"/>
+    </row>
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I38:J38"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I47:J47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1566,6 +1732,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>